<commit_message>
Worksheet templates with formulas ready
</commit_message>
<xml_diff>
--- a/DailyReport_Template.xlsx
+++ b/DailyReport_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tv\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3E98485D-44B5-4C95-9193-B70212F99253}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{93DAB620-9DAF-4D33-B873-1F11E83A3B78}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="4" xr2:uid="{25725CF7-E2D3-4635-80A8-0BAACCA8361A}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3327" uniqueCount="971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3903" uniqueCount="971">
   <si>
     <t>Column1</t>
   </si>
@@ -3217,9 +3217,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14513,27 +14516,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9BA1E8-795E-418B-A0CE-3B7E5F4CFA79}">
   <dimension ref="A1:P116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" customWidth="1"/>
-    <col min="10" max="10" width="31.5703125" customWidth="1"/>
-    <col min="11" max="11" width="39" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" customWidth="1"/>
+    <col min="12" max="12" width="31.5703125" customWidth="1"/>
+    <col min="13" max="13" width="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>968</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>969</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>970</v>
       </c>
       <c r="O1" t="s">
@@ -14556,29 +14561,31 @@
         <f>Sheet1!C5</f>
         <v>Order Time</v>
       </c>
-      <c r="D2" t="str">
-        <f>Sheet1!D5</f>
-        <v>Order Type</v>
-      </c>
-      <c r="E2" t="str">
-        <f>Sheet1!E5</f>
-        <v>Trade Description</v>
-      </c>
-      <c r="F2" t="str">
-        <f>Sheet1!F5</f>
-        <v>Account</v>
-      </c>
-      <c r="G2" t="str">
-        <f>Sheet1!G5</f>
-        <v>Quantity</v>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>630</v>
+      </c>
+      <c r="F2" t="s">
+        <v>631</v>
+      </c>
+      <c r="G2" t="s">
+        <v>632</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
       </c>
       <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
         <v>628</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>629</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>963</v>
       </c>
       <c r="O2" t="s">
@@ -14588,7 +14595,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>Sheet1!A6</f>
         <v>AVDL</v>
@@ -14603,24 +14610,26 @@
         <v>07:42:23 AM
 05/27/2022</v>
       </c>
-      <c r="D3" t="str">
-        <f>Sheet1!D6</f>
-        <v>Limit at $1.47</v>
-      </c>
-      <c r="E3" t="str">
-        <f>Sheet1!E6</f>
-        <v xml:space="preserve">Buy 100 Limit at $1.47  </v>
-      </c>
-      <c r="F3" t="str">
-        <f>Sheet1!F6</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G3" t="str">
-        <f>Sheet1!G6</f>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="G3" t="s">
+        <v>636</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>Sheet1!A7</f>
         <v>AVDL</v>
@@ -14635,24 +14644,26 @@
         <v>07:43:43 AM
 05/27/2022</v>
       </c>
-      <c r="D4" t="str">
-        <f>Sheet1!D7</f>
-        <v>Limit at $1.44</v>
-      </c>
-      <c r="E4" t="str">
-        <f>Sheet1!E7</f>
-        <v xml:space="preserve">Sell 100 Limit at $1.44  </v>
-      </c>
-      <c r="F4" t="str">
-        <f>Sheet1!F7</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G4" t="str">
-        <f>Sheet1!G7</f>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="G4" t="s">
+        <v>640</v>
+      </c>
+      <c r="H4" t="s">
+        <v>641</v>
+      </c>
+      <c r="I4">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>Sheet1!A8</f>
         <v>AVDL</v>
@@ -14667,24 +14678,26 @@
         <v>07:49:52 AM
 05/27/2022</v>
       </c>
-      <c r="D5" t="str">
-        <f>Sheet1!D8</f>
-        <v>Limit at $1.50</v>
-      </c>
-      <c r="E5" t="str">
-        <f>Sheet1!E8</f>
-        <v xml:space="preserve">Buy 100 Limit at $1.50  </v>
-      </c>
-      <c r="F5" t="str">
-        <f>Sheet1!F8</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G5" t="str">
-        <f>Sheet1!G8</f>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="G5" t="s">
+        <v>644</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>Sheet1!A9</f>
         <v>AVDL</v>
@@ -14699,24 +14712,26 @@
         <v>07:53:17 AM
 05/27/2022</v>
       </c>
-      <c r="D6" t="str">
-        <f>Sheet1!D9</f>
-        <v>Limit at $1.51</v>
-      </c>
-      <c r="E6" t="str">
-        <f>Sheet1!E9</f>
-        <v xml:space="preserve">Buy 100 Limit at $1.51  </v>
-      </c>
-      <c r="F6" t="str">
-        <f>Sheet1!F9</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G6" t="str">
-        <f>Sheet1!G9</f>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="G6" t="s">
+        <v>646</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>Sheet1!A10</f>
         <v>AVDL</v>
@@ -14731,24 +14746,26 @@
         <v>08:05:04 AM
 05/27/2022</v>
       </c>
-      <c r="D7" t="str">
-        <f>Sheet1!D10</f>
-        <v>Limit at $1.30</v>
-      </c>
-      <c r="E7" t="str">
-        <f>Sheet1!E10</f>
-        <v xml:space="preserve">Sell 100 Limit at $1.30  </v>
-      </c>
-      <c r="F7" t="str">
-        <f>Sheet1!F10</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G7" t="str">
-        <f>Sheet1!G10</f>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="G7" t="s">
+        <v>649</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>Sheet1!A11</f>
         <v>AVDL</v>
@@ -14763,24 +14780,26 @@
         <v>08:11:53 AM
 05/27/2022</v>
       </c>
-      <c r="D8" t="str">
-        <f>Sheet1!D11</f>
-        <v>Limit at $1.37</v>
-      </c>
-      <c r="E8" t="str">
-        <f>Sheet1!E11</f>
-        <v xml:space="preserve">Sell 100 Limit at $1.37  </v>
-      </c>
-      <c r="F8" t="str">
-        <f>Sheet1!F11</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G8" t="str">
-        <f>Sheet1!G11</f>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="G8" t="s">
+        <v>651</v>
+      </c>
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>Sheet1!A12</f>
         <v>AVDL</v>
@@ -14795,24 +14814,26 @@
         <v>08:12:40 AM
 05/27/2022</v>
       </c>
-      <c r="D9" t="str">
-        <f>Sheet1!D12</f>
-        <v>Limit at $1.52</v>
-      </c>
-      <c r="E9" t="str">
-        <f>Sheet1!E12</f>
-        <v xml:space="preserve">Buy 100 Limit at $1.52  </v>
-      </c>
-      <c r="F9" t="str">
-        <f>Sheet1!F12</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G9" t="str">
-        <f>Sheet1!G12</f>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="G9" t="s">
+        <v>654</v>
+      </c>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>Sheet1!A13</f>
         <v>AVDL</v>
@@ -14827,24 +14848,26 @@
         <v>08:14:42 AM
 05/27/2022</v>
       </c>
-      <c r="D10" t="str">
-        <f>Sheet1!D13</f>
-        <v>Limit at $1.51</v>
-      </c>
-      <c r="E10" t="str">
-        <f>Sheet1!E13</f>
-        <v xml:space="preserve">Buy 50 Limit at $1.51  </v>
-      </c>
-      <c r="F10" t="str">
-        <f>Sheet1!F13</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G10" t="str">
-        <f>Sheet1!G13</f>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="G10" t="s">
+        <v>646</v>
+      </c>
+      <c r="H10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>Sheet1!A14</f>
         <v>AVDL</v>
@@ -14859,24 +14882,26 @@
         <v>08:15:37 AM
 05/27/2022</v>
       </c>
-      <c r="D11" t="str">
-        <f>Sheet1!D14</f>
-        <v>Limit at $1.41</v>
-      </c>
-      <c r="E11" t="str">
-        <f>Sheet1!E14</f>
-        <v xml:space="preserve">Sell 100 Limit at $1.41  </v>
-      </c>
-      <c r="F11" t="str">
-        <f>Sheet1!F14</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G11" t="str">
-        <f>Sheet1!G14</f>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="G11" t="s">
+        <v>658</v>
+      </c>
+      <c r="H11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>Sheet1!A15</f>
         <v>AVDL</v>
@@ -14891,24 +14916,26 @@
         <v>08:16:05 AM
 05/27/2022</v>
       </c>
-      <c r="D12" t="str">
-        <f>Sheet1!D15</f>
-        <v>Limit at $1.44</v>
-      </c>
-      <c r="E12" t="str">
-        <f>Sheet1!E15</f>
-        <v xml:space="preserve">Sell 50 Limit at $1.44  </v>
-      </c>
-      <c r="F12" t="str">
-        <f>Sheet1!F15</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G12" t="str">
-        <f>Sheet1!G15</f>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="G12" t="s">
+        <v>640</v>
+      </c>
+      <c r="H12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>Sheet1!A16</f>
         <v>AVDL</v>
@@ -14923,24 +14950,26 @@
         <v>08:16:27 AM
 05/27/2022</v>
       </c>
-      <c r="D13" t="str">
-        <f>Sheet1!D16</f>
-        <v>Limit at $1.56</v>
-      </c>
-      <c r="E13" t="str">
-        <f>Sheet1!E16</f>
-        <v xml:space="preserve">Buy 100 Limit at $1.56  </v>
-      </c>
-      <c r="F13" t="str">
-        <f>Sheet1!F16</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G13" t="str">
-        <f>Sheet1!G16</f>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="G13" t="s">
+        <v>662</v>
+      </c>
+      <c r="H13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>Sheet1!A17</f>
         <v>AVDL</v>
@@ -14955,24 +14984,26 @@
         <v>08:17:50 AM
 05/27/2022</v>
       </c>
-      <c r="D14" t="str">
-        <f>Sheet1!D17</f>
-        <v>Limit at $1.40</v>
-      </c>
-      <c r="E14" t="str">
-        <f>Sheet1!E17</f>
-        <v xml:space="preserve">Sell 100 Limit at $1.40  </v>
-      </c>
-      <c r="F14" t="str">
-        <f>Sheet1!F17</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G14" t="str">
-        <f>Sheet1!G17</f>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="G14" t="s">
+        <v>665</v>
+      </c>
+      <c r="H14" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>Sheet1!A18</f>
         <v>AVDL</v>
@@ -14987,24 +15018,26 @@
         <v>08:18:21 AM
 05/27/2022</v>
       </c>
-      <c r="D15" t="str">
-        <f>Sheet1!D18</f>
-        <v>Limit at $1.56</v>
-      </c>
-      <c r="E15" t="str">
-        <f>Sheet1!E18</f>
-        <v xml:space="preserve">Buy 100 Limit at $1.56  </v>
-      </c>
-      <c r="F15" t="str">
-        <f>Sheet1!F18</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G15" t="str">
-        <f>Sheet1!G18</f>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="G15" t="s">
+        <v>662</v>
+      </c>
+      <c r="H15" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>Sheet1!A19</f>
         <v>AMC</v>
@@ -15019,24 +15052,26 @@
         <v>08:26:47 AM
 05/27/2022</v>
       </c>
-      <c r="D16" t="str">
-        <f>Sheet1!D19</f>
-        <v>Limit at $12.47</v>
-      </c>
-      <c r="E16" t="str">
-        <f>Sheet1!E19</f>
-        <v xml:space="preserve">Buy 30 Limit at $12.47  </v>
-      </c>
-      <c r="F16" t="str">
-        <f>Sheet1!F19</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G16" t="str">
-        <f>Sheet1!G19</f>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="G16" t="s">
+        <v>669</v>
+      </c>
+      <c r="H16" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>Sheet1!A20</f>
         <v>AMC</v>
@@ -15051,24 +15086,26 @@
         <v>08:32:42 AM
 05/27/2022</v>
       </c>
-      <c r="D17" t="str">
-        <f>Sheet1!D20</f>
-        <v>Limit at $12.41</v>
-      </c>
-      <c r="E17" t="str">
-        <f>Sheet1!E20</f>
-        <v xml:space="preserve">Buy 20 Limit at $12.41  </v>
-      </c>
-      <c r="F17" t="str">
-        <f>Sheet1!F20</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G17" t="str">
-        <f>Sheet1!G20</f>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="G17" t="s">
+        <v>672</v>
+      </c>
+      <c r="H17" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>Sheet1!A21</f>
         <v>SIGA</v>
@@ -15083,24 +15120,26 @@
         <v>08:36:23 AM
 05/27/2022</v>
       </c>
-      <c r="D18" t="str">
-        <f>Sheet1!D21</f>
-        <v>Limit at $10.87</v>
-      </c>
-      <c r="E18" t="str">
-        <f>Sheet1!E21</f>
-        <v xml:space="preserve">Buy 100 Limit at $10.87  </v>
-      </c>
-      <c r="F18" t="str">
-        <f>Sheet1!F21</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G18" t="str">
-        <f>Sheet1!G21</f>
+      <c r="D18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="G18" t="s">
+        <v>675</v>
+      </c>
+      <c r="H18" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>Sheet1!A22</f>
         <v>SIGA</v>
@@ -15115,24 +15154,26 @@
         <v>08:40:55 AM
 05/27/2022</v>
       </c>
-      <c r="D19" t="str">
-        <f>Sheet1!D22</f>
-        <v>Limit at $10.60</v>
-      </c>
-      <c r="E19" t="str">
-        <f>Sheet1!E22</f>
-        <v xml:space="preserve">Sell 50 Limit at $10.60  </v>
-      </c>
-      <c r="F19" t="str">
-        <f>Sheet1!F22</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G19" t="str">
-        <f>Sheet1!G22</f>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="G19" t="s">
+        <v>678</v>
+      </c>
+      <c r="H19" t="s">
+        <v>70</v>
+      </c>
+      <c r="I19">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>Sheet1!A23</f>
         <v>SIGA</v>
@@ -15147,24 +15188,26 @@
         <v>08:41:27 AM
 05/27/2022</v>
       </c>
-      <c r="D20" t="str">
-        <f>Sheet1!D23</f>
-        <v>Limit at $10.91</v>
-      </c>
-      <c r="E20" t="str">
-        <f>Sheet1!E23</f>
-        <v xml:space="preserve">Sell 50 Limit at $10.91  </v>
-      </c>
-      <c r="F20" t="str">
-        <f>Sheet1!F23</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G20" t="str">
-        <f>Sheet1!G23</f>
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="G20" t="s">
+        <v>681</v>
+      </c>
+      <c r="H20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I20">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>Sheet1!A24</f>
         <v>AMC</v>
@@ -15179,24 +15222,26 @@
         <v>08:44:08 AM
 05/27/2022</v>
       </c>
-      <c r="D21" t="str">
-        <f>Sheet1!D24</f>
-        <v>Limit at $12.42</v>
-      </c>
-      <c r="E21" t="str">
-        <f>Sheet1!E24</f>
-        <v xml:space="preserve">Sell 30 Limit at $12.42  </v>
-      </c>
-      <c r="F21" t="str">
-        <f>Sheet1!F24</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G21" t="str">
-        <f>Sheet1!G24</f>
+      <c r="D21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="G21" t="s">
+        <v>684</v>
+      </c>
+      <c r="H21" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>Sheet1!A25</f>
         <v>AVDL</v>
@@ -15211,24 +15256,26 @@
         <v>08:44:17 AM
 05/27/2022</v>
       </c>
-      <c r="D22" t="str">
-        <f>Sheet1!D25</f>
-        <v>Limit at $1.30</v>
-      </c>
-      <c r="E22" t="str">
-        <f>Sheet1!E25</f>
-        <v xml:space="preserve">Sell 100 Limit at $1.30  </v>
-      </c>
-      <c r="F22" t="str">
-        <f>Sheet1!F25</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G22" t="str">
-        <f>Sheet1!G25</f>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="G22" t="s">
+        <v>649</v>
+      </c>
+      <c r="H22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22">
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>Sheet1!A26</f>
         <v>AMC</v>
@@ -15243,24 +15290,26 @@
         <v>08:51:06 AM
 05/27/2022</v>
       </c>
-      <c r="D23" t="str">
-        <f>Sheet1!D26</f>
-        <v>Limit at $12.79</v>
-      </c>
-      <c r="E23" t="str">
-        <f>Sheet1!E26</f>
-        <v xml:space="preserve">Buy 30 Limit at $12.79  </v>
-      </c>
-      <c r="F23" t="str">
-        <f>Sheet1!F26</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G23" t="str">
-        <f>Sheet1!G26</f>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="G23" t="s">
+        <v>689</v>
+      </c>
+      <c r="H23" t="s">
+        <v>82</v>
+      </c>
+      <c r="I23">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>Sheet1!A27</f>
         <v>AMC</v>
@@ -15275,24 +15324,26 @@
         <v>08:53:53 AM
 05/27/2022</v>
       </c>
-      <c r="D24" t="str">
-        <f>Sheet1!D27</f>
-        <v>Limit at $12.62</v>
-      </c>
-      <c r="E24" t="str">
-        <f>Sheet1!E27</f>
-        <v xml:space="preserve">Buy 20 Limit at $12.62  </v>
-      </c>
-      <c r="F24" t="str">
-        <f>Sheet1!F27</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G24" t="str">
-        <f>Sheet1!G27</f>
+      <c r="D24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="G24" t="s">
+        <v>692</v>
+      </c>
+      <c r="H24" t="s">
+        <v>85</v>
+      </c>
+      <c r="I24">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>Sheet1!A28</f>
         <v>AVDL</v>
@@ -15307,24 +15358,26 @@
         <v>09:08:38 AM
 05/27/2022</v>
       </c>
-      <c r="D25" t="str">
-        <f>Sheet1!D28</f>
-        <v>Limit at $1.71</v>
-      </c>
-      <c r="E25" t="str">
-        <f>Sheet1!E28</f>
-        <v xml:space="preserve">Buy 100 Limit at $1.71  </v>
-      </c>
-      <c r="F25" t="str">
-        <f>Sheet1!F28</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G25" t="str">
-        <f>Sheet1!G28</f>
+      <c r="D25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="G25" t="s">
+        <v>695</v>
+      </c>
+      <c r="H25" t="s">
+        <v>88</v>
+      </c>
+      <c r="I25">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>Sheet1!A29</f>
         <v>AVDL</v>
@@ -15339,24 +15392,26 @@
         <v>09:11:26 AM
 05/27/2022</v>
       </c>
-      <c r="D26" t="str">
-        <f>Sheet1!D29</f>
-        <v>Limit at $1.50</v>
-      </c>
-      <c r="E26" t="str">
-        <f>Sheet1!E29</f>
-        <v xml:space="preserve">Sell 50 Limit at $1.50  </v>
-      </c>
-      <c r="F26" t="str">
-        <f>Sheet1!F29</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G26" t="str">
-        <f>Sheet1!G29</f>
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="G26" t="s">
+        <v>644</v>
+      </c>
+      <c r="H26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I26">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>Sheet1!A30</f>
         <v>AVDL</v>
@@ -15371,24 +15426,26 @@
         <v>09:12:29 AM
 05/27/2022</v>
       </c>
-      <c r="D27" t="str">
-        <f>Sheet1!D30</f>
-        <v>Limit at $1.65</v>
-      </c>
-      <c r="E27" t="str">
-        <f>Sheet1!E30</f>
-        <v xml:space="preserve">Sell 50 Limit at $1.65  </v>
-      </c>
-      <c r="F27" t="str">
-        <f>Sheet1!F30</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G27" t="str">
-        <f>Sheet1!G30</f>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="G27" t="s">
+        <v>700</v>
+      </c>
+      <c r="H27" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>Sheet1!A31</f>
         <v>AMC</v>
@@ -15403,24 +15460,26 @@
         <v>09:13:33 AM
 05/27/2022</v>
       </c>
-      <c r="D28" t="str">
-        <f>Sheet1!D31</f>
-        <v>Limit at $12.56</v>
-      </c>
-      <c r="E28" t="str">
-        <f>Sheet1!E31</f>
-        <v xml:space="preserve">Sell 50 Limit at $12.56  </v>
-      </c>
-      <c r="F28" t="str">
-        <f>Sheet1!F31</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G28" t="str">
-        <f>Sheet1!G31</f>
+      <c r="D28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="G28" t="s">
+        <v>703</v>
+      </c>
+      <c r="H28" t="s">
+        <v>97</v>
+      </c>
+      <c r="I28">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>Sheet1!A32</f>
         <v>MSFT</v>
@@ -15435,24 +15494,26 @@
         <v>09:35:49 AM
 05/27/2022</v>
       </c>
-      <c r="D29" t="str">
-        <f>Sheet1!D32</f>
-        <v>Limit at $269.38</v>
-      </c>
-      <c r="E29" t="str">
-        <f>Sheet1!E32</f>
-        <v xml:space="preserve">Buy 3 Limit at $269.38  </v>
-      </c>
-      <c r="F29" t="str">
-        <f>Sheet1!F32</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G29" t="str">
-        <f>Sheet1!G32</f>
+      <c r="D29" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="G29" t="s">
+        <v>706</v>
+      </c>
+      <c r="H29" t="s">
+        <v>101</v>
+      </c>
+      <c r="I29">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>Sheet1!A33</f>
         <v>AMD</v>
@@ -15467,24 +15528,26 @@
         <v>09:36:09 AM
 05/27/2022</v>
       </c>
-      <c r="D30" t="str">
-        <f>Sheet1!D33</f>
-        <v>Limit at $101.83</v>
-      </c>
-      <c r="E30" t="str">
-        <f>Sheet1!E33</f>
-        <v xml:space="preserve">Buy 3 Limit at $101.83  </v>
-      </c>
-      <c r="F30" t="str">
-        <f>Sheet1!F33</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G30" t="str">
-        <f>Sheet1!G33</f>
+      <c r="D30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="G30" t="s">
+        <v>709</v>
+      </c>
+      <c r="H30" t="s">
+        <v>106</v>
+      </c>
+      <c r="I30">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>Sheet1!A34</f>
         <v>TSLA</v>
@@ -15499,24 +15562,26 @@
         <v>09:36:22 AM
 05/27/2022</v>
       </c>
-      <c r="D31" t="str">
-        <f>Sheet1!D34</f>
-        <v>Limit at $736.00</v>
-      </c>
-      <c r="E31" t="str">
-        <f>Sheet1!E34</f>
-        <v xml:space="preserve">Buy 1 Limit at $736.00  </v>
-      </c>
-      <c r="F31" t="str">
-        <f>Sheet1!F34</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G31" t="str">
-        <f>Sheet1!G34</f>
+      <c r="D31" t="s">
+        <v>109</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="G31" t="s">
+        <v>712</v>
+      </c>
+      <c r="H31" t="s">
+        <v>110</v>
+      </c>
+      <c r="I31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>Sheet1!A35</f>
         <v>NVDA</v>
@@ -15531,24 +15596,26 @@
         <v>09:36:33 AM
 05/27/2022</v>
       </c>
-      <c r="D32" t="str">
-        <f>Sheet1!D35</f>
-        <v>Limit at $184.85</v>
-      </c>
-      <c r="E32" t="str">
-        <f>Sheet1!E35</f>
-        <v xml:space="preserve">Buy 3 Limit at $184.85  </v>
-      </c>
-      <c r="F32" t="str">
-        <f>Sheet1!F35</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G32" t="str">
-        <f>Sheet1!G35</f>
+      <c r="D32" t="s">
+        <v>113</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="G32" t="s">
+        <v>715</v>
+      </c>
+      <c r="H32" t="s">
+        <v>114</v>
+      </c>
+      <c r="I32">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>Sheet1!A36</f>
         <v>NCLH</v>
@@ -15563,24 +15630,26 @@
         <v>09:37:21 AM
 05/27/2022</v>
       </c>
-      <c r="D33" t="str">
-        <f>Sheet1!D36</f>
-        <v>Limit at $15.88</v>
-      </c>
-      <c r="E33" t="str">
-        <f>Sheet1!E36</f>
-        <v xml:space="preserve">Buy 5 Limit at $15.88  </v>
-      </c>
-      <c r="F33" t="str">
-        <f>Sheet1!F36</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G33" t="str">
-        <f>Sheet1!G36</f>
+      <c r="D33" t="s">
+        <v>117</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="G33" t="s">
+        <v>718</v>
+      </c>
+      <c r="H33" t="s">
+        <v>118</v>
+      </c>
+      <c r="I33">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>Sheet1!A37</f>
         <v>NCLH</v>
@@ -15595,24 +15664,26 @@
         <v>09:38:08 AM
 05/27/2022</v>
       </c>
-      <c r="D34" t="str">
-        <f>Sheet1!D37</f>
-        <v>Limit at $15.80</v>
-      </c>
-      <c r="E34" t="str">
-        <f>Sheet1!E37</f>
-        <v xml:space="preserve">Buy 5 Limit at $15.80  </v>
-      </c>
-      <c r="F34" t="str">
-        <f>Sheet1!F37</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G34" t="str">
-        <f>Sheet1!G37</f>
+      <c r="D34" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>719</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="G34" t="s">
+        <v>721</v>
+      </c>
+      <c r="H34" t="s">
+        <v>122</v>
+      </c>
+      <c r="I34">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>Sheet1!A38</f>
         <v>CCL</v>
@@ -15627,24 +15698,26 @@
         <v>09:38:38 AM
 05/27/2022</v>
       </c>
-      <c r="D35" t="str">
-        <f>Sheet1!D38</f>
-        <v>Limit at $13.72</v>
-      </c>
-      <c r="E35" t="str">
-        <f>Sheet1!E38</f>
-        <v xml:space="preserve">Buy 50 Limit at $13.72  </v>
-      </c>
-      <c r="F35" t="str">
-        <f>Sheet1!F38</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G35" t="str">
-        <f>Sheet1!G38</f>
+      <c r="D35" t="s">
+        <v>125</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="G35" t="s">
+        <v>724</v>
+      </c>
+      <c r="H35" t="s">
+        <v>126</v>
+      </c>
+      <c r="I35">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>Sheet1!A39</f>
         <v>FB</v>
@@ -15659,24 +15732,26 @@
         <v>09:42:05 AM
 05/27/2022</v>
       </c>
-      <c r="D36" t="str">
-        <f>Sheet1!D39</f>
-        <v>Limit at $192.43</v>
-      </c>
-      <c r="E36" t="str">
-        <f>Sheet1!E39</f>
-        <v xml:space="preserve">Buy 3 Limit at $192.43  </v>
-      </c>
-      <c r="F36" t="str">
-        <f>Sheet1!F39</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G36" t="str">
-        <f>Sheet1!G39</f>
+      <c r="D36" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="G36" t="s">
+        <v>727</v>
+      </c>
+      <c r="H36" t="s">
+        <v>130</v>
+      </c>
+      <c r="I36">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>Sheet1!A40</f>
         <v>FB</v>
@@ -15691,24 +15766,26 @@
         <v>09:42:59 AM
 05/27/2022</v>
       </c>
-      <c r="D37" t="str">
-        <f>Sheet1!D40</f>
-        <v>Limit at $191.71</v>
-      </c>
-      <c r="E37" t="str">
-        <f>Sheet1!E40</f>
-        <v xml:space="preserve">Buy 2 Limit at $191.71  </v>
-      </c>
-      <c r="F37" t="str">
-        <f>Sheet1!F40</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G37" t="str">
-        <f>Sheet1!G40</f>
+      <c r="D37" t="s">
+        <v>129</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="G37" t="s">
+        <v>730</v>
+      </c>
+      <c r="H37" t="s">
+        <v>133</v>
+      </c>
+      <c r="I37">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>Sheet1!A41</f>
         <v>AMD</v>
@@ -15723,24 +15800,26 @@
         <v>09:45:34 AM
 05/27/2022</v>
       </c>
-      <c r="D38" t="str">
-        <f>Sheet1!D41</f>
-        <v>Limit at $99.99</v>
-      </c>
-      <c r="E38" t="str">
-        <f>Sheet1!E41</f>
-        <v xml:space="preserve">Buy 2 Limit at $99.99  </v>
-      </c>
-      <c r="F38" t="str">
-        <f>Sheet1!F41</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G38" t="str">
-        <f>Sheet1!G41</f>
+      <c r="D38" t="s">
+        <v>105</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="G38" t="s">
+        <v>733</v>
+      </c>
+      <c r="H38" t="s">
+        <v>137</v>
+      </c>
+      <c r="I38">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>Sheet1!A42</f>
         <v>NVDA</v>
@@ -15755,24 +15834,26 @@
         <v>09:46:29 AM
 05/27/2022</v>
       </c>
-      <c r="D39" t="str">
-        <f>Sheet1!D42</f>
-        <v>Limit at $182.72</v>
-      </c>
-      <c r="E39" t="str">
-        <f>Sheet1!E42</f>
-        <v xml:space="preserve">Buy 2 Limit at $182.72  </v>
-      </c>
-      <c r="F39" t="str">
-        <f>Sheet1!F42</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G39" t="str">
-        <f>Sheet1!G42</f>
+      <c r="D39" t="s">
+        <v>113</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="G39" t="s">
+        <v>736</v>
+      </c>
+      <c r="H39" t="s">
+        <v>140</v>
+      </c>
+      <c r="I39">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>Sheet1!A43</f>
         <v>AMC</v>
@@ -15787,24 +15868,26 @@
         <v>09:47:32 AM
 05/27/2022</v>
       </c>
-      <c r="D40" t="str">
-        <f>Sheet1!D43</f>
-        <v>Stop Loss at $12.55</v>
-      </c>
-      <c r="E40" t="str">
-        <f>Sheet1!E43</f>
-        <v xml:space="preserve">Sell 20 Stop Loss at $12.55  </v>
-      </c>
-      <c r="F40" t="str">
-        <f>Sheet1!F43</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G40" t="str">
-        <f>Sheet1!G43</f>
+      <c r="D40" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="G40" t="s">
+        <v>739</v>
+      </c>
+      <c r="H40" t="s">
+        <v>143</v>
+      </c>
+      <c r="I40">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>Sheet1!A44</f>
         <v>SHOP</v>
@@ -15819,24 +15902,26 @@
         <v>09:48:57 AM
 05/27/2022</v>
       </c>
-      <c r="D41" t="str">
-        <f>Sheet1!D44</f>
-        <v>Limit at $360.00</v>
-      </c>
-      <c r="E41" t="str">
-        <f>Sheet1!E44</f>
-        <v xml:space="preserve">Buy 1 Limit at $360.00  </v>
-      </c>
-      <c r="F41" t="str">
-        <f>Sheet1!F44</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G41" t="str">
-        <f>Sheet1!G44</f>
+      <c r="D41" t="s">
+        <v>147</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="G41" t="s">
+        <v>742</v>
+      </c>
+      <c r="H41" t="s">
+        <v>148</v>
+      </c>
+      <c r="I41">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>Sheet1!A45</f>
         <v>TSLA</v>
@@ -15851,24 +15936,26 @@
         <v>09:50:46 AM
 05/27/2022</v>
       </c>
-      <c r="D42" t="str">
-        <f>Sheet1!D45</f>
-        <v>Limit at $740.71</v>
-      </c>
-      <c r="E42" t="str">
-        <f>Sheet1!E45</f>
-        <v xml:space="preserve">Buy 1 Limit at $740.71  </v>
-      </c>
-      <c r="F42" t="str">
-        <f>Sheet1!F45</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G42" t="str">
-        <f>Sheet1!G45</f>
+      <c r="D42" t="s">
+        <v>109</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="G42" t="s">
+        <v>745</v>
+      </c>
+      <c r="H42" t="s">
+        <v>151</v>
+      </c>
+      <c r="I42">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>Sheet1!A46</f>
         <v>BABA</v>
@@ -15883,24 +15970,26 @@
         <v>09:51:40 AM
 05/27/2022</v>
       </c>
-      <c r="D43" t="str">
-        <f>Sheet1!D46</f>
-        <v>Limit at $91.78</v>
-      </c>
-      <c r="E43" t="str">
-        <f>Sheet1!E46</f>
-        <v xml:space="preserve">Buy 3 Limit at $91.78  </v>
-      </c>
-      <c r="F43" t="str">
-        <f>Sheet1!F46</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G43" t="str">
-        <f>Sheet1!G46</f>
+      <c r="D43" t="s">
+        <v>154</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>746</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="G43" t="s">
+        <v>748</v>
+      </c>
+      <c r="H43" t="s">
+        <v>155</v>
+      </c>
+      <c r="I43">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>Sheet1!A47</f>
         <v>RDBX</v>
@@ -15915,24 +16004,26 @@
         <v>09:54:40 AM
 05/27/2022</v>
       </c>
-      <c r="D44" t="str">
-        <f>Sheet1!D47</f>
-        <v>Limit at $8.33</v>
-      </c>
-      <c r="E44" t="str">
-        <f>Sheet1!E47</f>
-        <v xml:space="preserve">Buy 50 Limit at $8.33  </v>
-      </c>
-      <c r="F44" t="str">
-        <f>Sheet1!F47</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G44" t="str">
-        <f>Sheet1!G47</f>
+      <c r="D44" t="s">
+        <v>158</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="G44" t="s">
+        <v>751</v>
+      </c>
+      <c r="H44" t="s">
+        <v>159</v>
+      </c>
+      <c r="I44">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>Sheet1!A48</f>
         <v>RDBX</v>
@@ -15947,24 +16038,26 @@
         <v>10:01:10 AM
 05/27/2022</v>
       </c>
-      <c r="D45" t="str">
-        <f>Sheet1!D48</f>
-        <v>Market</v>
-      </c>
-      <c r="E45" t="str">
-        <f>Sheet1!E48</f>
-        <v xml:space="preserve">Sell 50 at Market  </v>
-      </c>
-      <c r="F45" t="str">
-        <f>Sheet1!F48</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G45" t="str">
-        <f>Sheet1!G48</f>
+      <c r="D45" t="s">
+        <v>158</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="G45" t="s">
+        <v>754</v>
+      </c>
+      <c r="H45" t="s">
+        <v>162</v>
+      </c>
+      <c r="I45">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>Sheet1!A49</f>
         <v>AMC</v>
@@ -15979,24 +16072,26 @@
         <v>10:02:31 AM
 05/27/2022</v>
       </c>
-      <c r="D46" t="str">
-        <f>Sheet1!D49</f>
-        <v>Limit at $12.88</v>
-      </c>
-      <c r="E46" t="str">
-        <f>Sheet1!E49</f>
-        <v xml:space="preserve">Buy 10 Limit at $12.88  </v>
-      </c>
-      <c r="F46" t="str">
-        <f>Sheet1!F49</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G46" t="str">
-        <f>Sheet1!G49</f>
+      <c r="D46" t="s">
+        <v>57</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="G46" t="s">
+        <v>757</v>
+      </c>
+      <c r="H46" t="s">
+        <v>165</v>
+      </c>
+      <c r="I46">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>Sheet1!A50</f>
         <v>AMC</v>
@@ -16011,24 +16106,26 @@
         <v>10:03:11 AM
 05/27/2022</v>
       </c>
-      <c r="D47" t="str">
-        <f>Sheet1!D50</f>
-        <v>Limit at $12.86</v>
-      </c>
-      <c r="E47" t="str">
-        <f>Sheet1!E50</f>
-        <v xml:space="preserve">Sell 10 Limit at $12.86  </v>
-      </c>
-      <c r="F47" t="str">
-        <f>Sheet1!F50</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G47" t="str">
-        <f>Sheet1!G50</f>
+      <c r="D47" t="s">
+        <v>57</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="G47" t="s">
+        <v>760</v>
+      </c>
+      <c r="H47" t="s">
+        <v>169</v>
+      </c>
+      <c r="I47">
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>Sheet1!A51</f>
         <v>AMC</v>
@@ -16043,24 +16140,26 @@
         <v>10:04:51 AM
 05/27/2022</v>
       </c>
-      <c r="D48" t="str">
-        <f>Sheet1!D51</f>
-        <v>Limit at $13.28</v>
-      </c>
-      <c r="E48" t="str">
-        <f>Sheet1!E51</f>
-        <v xml:space="preserve">Buy 10 Limit at $13.28  </v>
-      </c>
-      <c r="F48" t="str">
-        <f>Sheet1!F51</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G48" t="str">
-        <f>Sheet1!G51</f>
+      <c r="D48" t="s">
+        <v>57</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="G48" t="s">
+        <v>763</v>
+      </c>
+      <c r="H48" t="s">
+        <v>173</v>
+      </c>
+      <c r="I48">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>Sheet1!A52</f>
         <v>AMC</v>
@@ -16075,24 +16174,26 @@
         <v>10:05:32 AM
 05/27/2022</v>
       </c>
-      <c r="D49" t="str">
-        <f>Sheet1!D52</f>
-        <v>Limit at $13.10</v>
-      </c>
-      <c r="E49" t="str">
-        <f>Sheet1!E52</f>
-        <v xml:space="preserve">Sell 10 Limit at $13.10  </v>
-      </c>
-      <c r="F49" t="str">
-        <f>Sheet1!F52</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G49" t="str">
-        <f>Sheet1!G52</f>
+      <c r="D49" t="s">
+        <v>57</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="G49" t="s">
+        <v>766</v>
+      </c>
+      <c r="H49" t="s">
+        <v>176</v>
+      </c>
+      <c r="I49">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>Sheet1!A53</f>
         <v>MSFT</v>
@@ -16107,24 +16208,26 @@
         <v>10:10:03 AM
 05/27/2022</v>
       </c>
-      <c r="D50" t="str">
-        <f>Sheet1!D53</f>
-        <v>Limit at $271.45</v>
-      </c>
-      <c r="E50" t="str">
-        <f>Sheet1!E53</f>
-        <v xml:space="preserve">Buy 3 Limit at $271.45  </v>
-      </c>
-      <c r="F50" t="str">
-        <f>Sheet1!F53</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G50" t="str">
-        <f>Sheet1!G53</f>
+      <c r="D50" t="s">
+        <v>100</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="G50" t="s">
+        <v>769</v>
+      </c>
+      <c r="H50" t="s">
+        <v>179</v>
+      </c>
+      <c r="I50">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>Sheet1!A54</f>
         <v>MRNA</v>
@@ -16139,24 +16242,26 @@
         <v>10:14:13 AM
 05/27/2022</v>
       </c>
-      <c r="D51" t="str">
-        <f>Sheet1!D54</f>
-        <v>Limit at $142.89</v>
-      </c>
-      <c r="E51" t="str">
-        <f>Sheet1!E54</f>
-        <v xml:space="preserve">Buy 3 Limit at $142.89  </v>
-      </c>
-      <c r="F51" t="str">
-        <f>Sheet1!F54</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G51" t="str">
-        <f>Sheet1!G54</f>
+      <c r="D51" t="s">
+        <v>182</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="G51" t="s">
+        <v>772</v>
+      </c>
+      <c r="H51" t="s">
+        <v>183</v>
+      </c>
+      <c r="I51">
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>Sheet1!A55</f>
         <v>AMC</v>
@@ -16171,24 +16276,26 @@
         <v>10:14:31 AM
 05/27/2022</v>
       </c>
-      <c r="D52" t="str">
-        <f>Sheet1!D55</f>
-        <v>Limit at $13.90</v>
-      </c>
-      <c r="E52" t="str">
-        <f>Sheet1!E55</f>
-        <v xml:space="preserve">Buy 5 Limit at $13.90  </v>
-      </c>
-      <c r="F52" t="str">
-        <f>Sheet1!F55</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G52" t="str">
-        <f>Sheet1!G55</f>
+      <c r="D52" t="s">
+        <v>57</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>773</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>774</v>
+      </c>
+      <c r="G52" t="s">
+        <v>775</v>
+      </c>
+      <c r="H52" t="s">
+        <v>186</v>
+      </c>
+      <c r="I52">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>Sheet1!A56</f>
         <v>AMC</v>
@@ -16203,24 +16310,26 @@
         <v>10:16:12 AM
 05/27/2022</v>
       </c>
-      <c r="D53" t="str">
-        <f>Sheet1!D56</f>
-        <v>Limit at $13.33</v>
-      </c>
-      <c r="E53" t="str">
-        <f>Sheet1!E56</f>
-        <v xml:space="preserve">Buy 5 Limit at $13.33  </v>
-      </c>
-      <c r="F53" t="str">
-        <f>Sheet1!F56</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G53" t="str">
-        <f>Sheet1!G56</f>
+      <c r="D53" t="s">
+        <v>57</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>777</v>
+      </c>
+      <c r="G53" t="s">
+        <v>778</v>
+      </c>
+      <c r="H53" t="s">
+        <v>189</v>
+      </c>
+      <c r="I53">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>Sheet1!A57</f>
         <v>MRVL</v>
@@ -16235,24 +16344,26 @@
         <v>10:18:14 AM
 05/27/2022</v>
       </c>
-      <c r="D54" t="str">
-        <f>Sheet1!D57</f>
-        <v>Limit at $58.80</v>
-      </c>
-      <c r="E54" t="str">
-        <f>Sheet1!E57</f>
-        <v xml:space="preserve">Buy 1 Limit at $58.80  </v>
-      </c>
-      <c r="F54" t="str">
-        <f>Sheet1!F57</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G54" t="str">
-        <f>Sheet1!G57</f>
+      <c r="D54" t="s">
+        <v>192</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="G54" t="s">
+        <v>781</v>
+      </c>
+      <c r="H54" t="s">
+        <v>193</v>
+      </c>
+      <c r="I54">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>Sheet1!A58</f>
         <v>CCL</v>
@@ -16267,24 +16378,26 @@
         <v>10:20:43 AM
 05/27/2022</v>
       </c>
-      <c r="D55" t="str">
-        <f>Sheet1!D58</f>
-        <v>Stop Loss at $13.48</v>
-      </c>
-      <c r="E55" t="str">
-        <f>Sheet1!E58</f>
-        <v xml:space="preserve">Sell 50 Stop Loss at $13.48  </v>
-      </c>
-      <c r="F55" t="str">
-        <f>Sheet1!F58</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G55" t="str">
-        <f>Sheet1!G58</f>
+      <c r="D55" t="s">
+        <v>125</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="G55" t="s">
+        <v>784</v>
+      </c>
+      <c r="H55" t="s">
+        <v>196</v>
+      </c>
+      <c r="I55">
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f>Sheet1!A59</f>
         <v>NVDA</v>
@@ -16299,24 +16412,26 @@
         <v>10:21:57 AM
 05/27/2022</v>
       </c>
-      <c r="D56" t="str">
-        <f>Sheet1!D59</f>
-        <v>Limit at $186.26</v>
-      </c>
-      <c r="E56" t="str">
-        <f>Sheet1!E59</f>
-        <v xml:space="preserve">Buy 2 Limit at $186.26  </v>
-      </c>
-      <c r="F56" t="str">
-        <f>Sheet1!F59</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G56" t="str">
-        <f>Sheet1!G59</f>
+      <c r="D56" t="s">
+        <v>113</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="G56" t="s">
+        <v>787</v>
+      </c>
+      <c r="H56" t="s">
+        <v>199</v>
+      </c>
+      <c r="I56">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f>Sheet1!A60</f>
         <v>BABA</v>
@@ -16331,24 +16446,26 @@
         <v>10:27:35 AM
 05/27/2022</v>
       </c>
-      <c r="D57" t="str">
-        <f>Sheet1!D60</f>
-        <v>Limit at $92.53</v>
-      </c>
-      <c r="E57" t="str">
-        <f>Sheet1!E60</f>
-        <v xml:space="preserve">Buy 1 Limit at $92.53  </v>
-      </c>
-      <c r="F57" t="str">
-        <f>Sheet1!F60</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G57" t="str">
-        <f>Sheet1!G60</f>
+      <c r="D57" t="s">
+        <v>154</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="G57" t="s">
+        <v>790</v>
+      </c>
+      <c r="H57" t="s">
+        <v>202</v>
+      </c>
+      <c r="I57">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f>Sheet1!A61</f>
         <v>AMC</v>
@@ -16363,24 +16480,26 @@
         <v>10:28:12 AM
 05/27/2022</v>
       </c>
-      <c r="D58" t="str">
-        <f>Sheet1!D61</f>
-        <v>Limit at $12.95</v>
-      </c>
-      <c r="E58" t="str">
-        <f>Sheet1!E61</f>
-        <v xml:space="preserve">Buy 10 Limit at $12.95  </v>
-      </c>
-      <c r="F58" t="str">
-        <f>Sheet1!F61</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G58" t="str">
-        <f>Sheet1!G61</f>
+      <c r="D58" t="s">
+        <v>57</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="G58" t="s">
+        <v>793</v>
+      </c>
+      <c r="H58" t="s">
+        <v>205</v>
+      </c>
+      <c r="I58">
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f>Sheet1!A62</f>
         <v>NVDA</v>
@@ -16395,24 +16514,26 @@
         <v>10:30:54 AM
 05/27/2022</v>
       </c>
-      <c r="D59" t="str">
-        <f>Sheet1!D62</f>
-        <v>Limit at $185.00</v>
-      </c>
-      <c r="E59" t="str">
-        <f>Sheet1!E62</f>
-        <v xml:space="preserve">Buy 1 Limit at $185.00  </v>
-      </c>
-      <c r="F59" t="str">
-        <f>Sheet1!F62</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G59" t="str">
-        <f>Sheet1!G62</f>
+      <c r="D59" t="s">
+        <v>113</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="G59" t="s">
+        <v>796</v>
+      </c>
+      <c r="H59" t="s">
+        <v>208</v>
+      </c>
+      <c r="I59">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f>Sheet1!A63</f>
         <v>SHOP</v>
@@ -16427,24 +16548,26 @@
         <v>10:32:13 AM
 05/27/2022</v>
       </c>
-      <c r="D60" t="str">
-        <f>Sheet1!D63</f>
-        <v>Limit at $364.68</v>
-      </c>
-      <c r="E60" t="str">
-        <f>Sheet1!E63</f>
-        <v xml:space="preserve">Buy 1 Limit at $364.68  </v>
-      </c>
-      <c r="F60" t="str">
-        <f>Sheet1!F63</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G60" t="str">
-        <f>Sheet1!G63</f>
+      <c r="D60" t="s">
+        <v>147</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="G60" t="s">
+        <v>799</v>
+      </c>
+      <c r="H60" t="s">
+        <v>211</v>
+      </c>
+      <c r="I60">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f>Sheet1!A64</f>
         <v>TSLA</v>
@@ -16459,24 +16582,26 @@
         <v>10:32:37 AM
 05/27/2022</v>
       </c>
-      <c r="D61" t="str">
-        <f>Sheet1!D64</f>
-        <v>Limit at $749.20</v>
-      </c>
-      <c r="E61" t="str">
-        <f>Sheet1!E64</f>
-        <v xml:space="preserve">Buy 1 Limit at $749.20  </v>
-      </c>
-      <c r="F61" t="str">
-        <f>Sheet1!F64</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G61" t="str">
-        <f>Sheet1!G64</f>
+      <c r="D61" t="s">
+        <v>109</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="G61" t="s">
+        <v>802</v>
+      </c>
+      <c r="H61" t="s">
+        <v>214</v>
+      </c>
+      <c r="I61">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f>Sheet1!A65</f>
         <v>MRNA</v>
@@ -16491,24 +16616,26 @@
         <v>10:34:34 AM
 05/27/2022</v>
       </c>
-      <c r="D62" t="str">
-        <f>Sheet1!D65</f>
-        <v>Limit at $144.55</v>
-      </c>
-      <c r="E62" t="str">
-        <f>Sheet1!E65</f>
-        <v xml:space="preserve">Buy 1 Limit at $144.55  </v>
-      </c>
-      <c r="F62" t="str">
-        <f>Sheet1!F65</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G62" t="str">
-        <f>Sheet1!G65</f>
+      <c r="D62" t="s">
+        <v>182</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="G62" t="s">
+        <v>805</v>
+      </c>
+      <c r="H62" t="s">
+        <v>217</v>
+      </c>
+      <c r="I62">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f>Sheet1!A66</f>
         <v>MRNA</v>
@@ -16523,24 +16650,26 @@
         <v>10:36:33 AM
 05/27/2022</v>
       </c>
-      <c r="D63" t="str">
-        <f>Sheet1!D66</f>
-        <v>Limit at $143.90</v>
-      </c>
-      <c r="E63" t="str">
-        <f>Sheet1!E66</f>
-        <v xml:space="preserve">Buy 1 Limit at $143.90  </v>
-      </c>
-      <c r="F63" t="str">
-        <f>Sheet1!F66</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G63" t="str">
-        <f>Sheet1!G66</f>
+      <c r="D63" t="s">
+        <v>182</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="G63" t="s">
+        <v>808</v>
+      </c>
+      <c r="H63" t="s">
+        <v>220</v>
+      </c>
+      <c r="I63">
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f>Sheet1!A67</f>
         <v>SQ</v>
@@ -16555,24 +16684,26 @@
         <v>10:41:45 AM
 05/27/2022</v>
       </c>
-      <c r="D64" t="str">
-        <f>Sheet1!D67</f>
-        <v>Limit at $89.56</v>
-      </c>
-      <c r="E64" t="str">
-        <f>Sheet1!E67</f>
-        <v xml:space="preserve">Buy 1 Limit at $89.56  </v>
-      </c>
-      <c r="F64" t="str">
-        <f>Sheet1!F67</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G64" t="str">
-        <f>Sheet1!G67</f>
+      <c r="D64" t="s">
+        <v>223</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>809</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="G64" t="s">
+        <v>811</v>
+      </c>
+      <c r="H64" t="s">
+        <v>224</v>
+      </c>
+      <c r="I64">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f>Sheet1!A68</f>
         <v>MRNA</v>
@@ -16587,24 +16718,26 @@
         <v>10:46:59 AM
 05/27/2022</v>
       </c>
-      <c r="D65" t="str">
-        <f>Sheet1!D68</f>
-        <v>Limit at $143.20</v>
-      </c>
-      <c r="E65" t="str">
-        <f>Sheet1!E68</f>
-        <v xml:space="preserve">Buy 1 Limit at $143.20  </v>
-      </c>
-      <c r="F65" t="str">
-        <f>Sheet1!F68</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G65" t="str">
-        <f>Sheet1!G68</f>
+      <c r="D65" t="s">
+        <v>182</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="G65" t="s">
+        <v>814</v>
+      </c>
+      <c r="H65" t="s">
+        <v>227</v>
+      </c>
+      <c r="I65">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f>Sheet1!A69</f>
         <v>AVDL</v>
@@ -16619,24 +16752,26 @@
         <v>10:52:20 AM
 05/27/2022</v>
       </c>
-      <c r="D66" t="str">
-        <f>Sheet1!D69</f>
-        <v>Limit at $2.37</v>
-      </c>
-      <c r="E66" t="str">
-        <f>Sheet1!E69</f>
-        <v xml:space="preserve">Buy 100 Limit at $2.37  </v>
-      </c>
-      <c r="F66" t="str">
-        <f>Sheet1!F69</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G66" t="str">
-        <f>Sheet1!G69</f>
+      <c r="D66" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="G66" t="s">
+        <v>817</v>
+      </c>
+      <c r="H66" t="s">
+        <v>230</v>
+      </c>
+      <c r="I66">
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f>Sheet1!A70</f>
         <v>AVDL</v>
@@ -16651,24 +16786,26 @@
         <v>10:55:40 AM
 05/27/2022</v>
       </c>
-      <c r="D67" t="str">
-        <f>Sheet1!D70</f>
-        <v>Limit at $2.32</v>
-      </c>
-      <c r="E67" t="str">
-        <f>Sheet1!E70</f>
-        <v xml:space="preserve">Buy 20 Limit at $2.32  </v>
-      </c>
-      <c r="F67" t="str">
-        <f>Sheet1!F70</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G67" t="str">
-        <f>Sheet1!G70</f>
+      <c r="D67" t="s">
+        <v>17</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="G67" t="s">
+        <v>820</v>
+      </c>
+      <c r="H67" t="s">
+        <v>233</v>
+      </c>
+      <c r="I67">
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f>Sheet1!A71</f>
         <v>AVDL</v>
@@ -16683,24 +16820,26 @@
         <v>10:56:07 AM
 05/27/2022</v>
       </c>
-      <c r="D68" t="str">
-        <f>Sheet1!D71</f>
-        <v>Limit at $2.30</v>
-      </c>
-      <c r="E68" t="str">
-        <f>Sheet1!E71</f>
-        <v xml:space="preserve">Buy 30 Limit at $2.30  </v>
-      </c>
-      <c r="F68" t="str">
-        <f>Sheet1!F71</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G68" t="str">
-        <f>Sheet1!G71</f>
+      <c r="D68" t="s">
+        <v>17</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="G68" t="s">
+        <v>823</v>
+      </c>
+      <c r="H68" t="s">
+        <v>236</v>
+      </c>
+      <c r="I68">
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f>Sheet1!A72</f>
         <v>IMTE</v>
@@ -16715,24 +16854,26 @@
         <v>11:12:53 AM
 05/27/2022</v>
       </c>
-      <c r="D69" t="str">
-        <f>Sheet1!D72</f>
-        <v>Limit at $8.78</v>
-      </c>
-      <c r="E69" t="str">
-        <f>Sheet1!E72</f>
-        <v xml:space="preserve">Buy 50 Limit at $8.78  </v>
-      </c>
-      <c r="F69" t="str">
-        <f>Sheet1!F72</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G69" t="str">
-        <f>Sheet1!G72</f>
+      <c r="D69" t="s">
+        <v>239</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>824</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="G69" t="s">
+        <v>826</v>
+      </c>
+      <c r="H69" t="s">
+        <v>240</v>
+      </c>
+      <c r="I69">
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f>Sheet1!A73</f>
         <v>IMTE</v>
@@ -16747,24 +16888,26 @@
         <v>11:13:19 AM
 05/27/2022</v>
       </c>
-      <c r="D70" t="str">
-        <f>Sheet1!D73</f>
-        <v>Limit at $8.90</v>
-      </c>
-      <c r="E70" t="str">
-        <f>Sheet1!E73</f>
-        <v xml:space="preserve">Buy 50 Limit at $8.90  </v>
-      </c>
-      <c r="F70" t="str">
-        <f>Sheet1!F73</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G70" t="str">
-        <f>Sheet1!G73</f>
+      <c r="D70" t="s">
+        <v>239</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="G70" t="s">
+        <v>829</v>
+      </c>
+      <c r="H70" t="s">
+        <v>243</v>
+      </c>
+      <c r="I70">
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f>Sheet1!A74</f>
         <v>IMTE</v>
@@ -16779,24 +16922,26 @@
         <v>11:13:59 AM
 05/27/2022</v>
       </c>
-      <c r="D71" t="str">
-        <f>Sheet1!D74</f>
-        <v>Stop Loss at $8.48</v>
-      </c>
-      <c r="E71" t="str">
-        <f>Sheet1!E74</f>
-        <v xml:space="preserve">Sell 100 Stop Loss at $8.48  </v>
-      </c>
-      <c r="F71" t="str">
-        <f>Sheet1!F74</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G71" t="str">
-        <f>Sheet1!G74</f>
+      <c r="D71" t="s">
+        <v>239</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="G71" t="s">
+        <v>832</v>
+      </c>
+      <c r="H71" t="s">
+        <v>246</v>
+      </c>
+      <c r="I71">
         <v>100</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f>Sheet1!A75</f>
         <v>AVDL</v>
@@ -16811,24 +16956,26 @@
         <v>11:16:33 AM
 05/27/2022</v>
       </c>
-      <c r="D72" t="str">
-        <f>Sheet1!D75</f>
-        <v>Market</v>
-      </c>
-      <c r="E72" t="str">
-        <f>Sheet1!E75</f>
-        <v xml:space="preserve">Sell 50 at Market  </v>
-      </c>
-      <c r="F72" t="str">
-        <f>Sheet1!F75</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G72" t="str">
-        <f>Sheet1!G75</f>
+      <c r="D72" t="s">
+        <v>17</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="G72" t="s">
+        <v>754</v>
+      </c>
+      <c r="H72" t="s">
+        <v>162</v>
+      </c>
+      <c r="I72">
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f>Sheet1!A76</f>
         <v>IMTE</v>
@@ -16843,24 +16990,26 @@
         <v>11:20:50 AM
 05/27/2022</v>
       </c>
-      <c r="D73" t="str">
-        <f>Sheet1!D76</f>
-        <v>Limit at $8.81</v>
-      </c>
-      <c r="E73" t="str">
-        <f>Sheet1!E76</f>
-        <v xml:space="preserve">Buy 30 Limit at $8.81  </v>
-      </c>
-      <c r="F73" t="str">
-        <f>Sheet1!F76</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G73" t="str">
-        <f>Sheet1!G76</f>
+      <c r="D73" t="s">
+        <v>239</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>824</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="G73" t="s">
+        <v>836</v>
+      </c>
+      <c r="H73" t="s">
+        <v>251</v>
+      </c>
+      <c r="I73">
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f>Sheet1!A77</f>
         <v>AVDL</v>
@@ -16875,24 +17024,26 @@
         <v>11:21:11 AM
 05/27/2022</v>
       </c>
-      <c r="D74" t="str">
-        <f>Sheet1!D77</f>
-        <v>Limit at $2.36</v>
-      </c>
-      <c r="E74" t="str">
-        <f>Sheet1!E77</f>
-        <v xml:space="preserve">Sell 100 Limit at $2.36  </v>
-      </c>
-      <c r="F74" t="str">
-        <f>Sheet1!F77</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G74" t="str">
-        <f>Sheet1!G77</f>
+      <c r="D74" t="s">
+        <v>17</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>837</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="G74" t="s">
+        <v>839</v>
+      </c>
+      <c r="H74" t="s">
+        <v>253</v>
+      </c>
+      <c r="I74">
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f>Sheet1!A78</f>
         <v>AVDL</v>
@@ -16907,24 +17058,26 @@
         <v>11:22:37 AM
 05/27/2022</v>
       </c>
-      <c r="D75" t="str">
-        <f>Sheet1!D78</f>
-        <v>Limit at $2.63</v>
-      </c>
-      <c r="E75" t="str">
-        <f>Sheet1!E78</f>
-        <v xml:space="preserve">Buy 100 Limit at $2.63  </v>
-      </c>
-      <c r="F75" t="str">
-        <f>Sheet1!F78</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G75" t="str">
-        <f>Sheet1!G78</f>
+      <c r="D75" t="s">
+        <v>17</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="G75" t="s">
+        <v>842</v>
+      </c>
+      <c r="H75" t="s">
+        <v>256</v>
+      </c>
+      <c r="I75">
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f>Sheet1!A79</f>
         <v>SIGA</v>
@@ -16939,24 +17092,26 @@
         <v>11:26:32 AM
 05/27/2022</v>
       </c>
-      <c r="D76" t="str">
-        <f>Sheet1!D79</f>
-        <v>Limit at $11.90</v>
-      </c>
-      <c r="E76" t="str">
-        <f>Sheet1!E79</f>
-        <v xml:space="preserve">Buy 50 Limit at $11.90  </v>
-      </c>
-      <c r="F76" t="str">
-        <f>Sheet1!F79</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G76" t="str">
-        <f>Sheet1!G79</f>
+      <c r="D76" t="s">
+        <v>66</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="G76" t="s">
+        <v>845</v>
+      </c>
+      <c r="H76" t="s">
+        <v>259</v>
+      </c>
+      <c r="I76">
         <v>50</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f>Sheet1!A80</f>
         <v>IMTE</v>
@@ -16971,24 +17126,26 @@
         <v>11:28:32 AM
 05/27/2022</v>
       </c>
-      <c r="D77" t="str">
-        <f>Sheet1!D80</f>
-        <v>Limit at $8.60</v>
-      </c>
-      <c r="E77" t="str">
-        <f>Sheet1!E80</f>
-        <v xml:space="preserve">Sell 30 Limit at $8.60  </v>
-      </c>
-      <c r="F77" t="str">
-        <f>Sheet1!F80</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G77" t="str">
-        <f>Sheet1!G80</f>
+      <c r="D77" t="s">
+        <v>239</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="G77" t="s">
+        <v>848</v>
+      </c>
+      <c r="H77" t="s">
+        <v>262</v>
+      </c>
+      <c r="I77">
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f>Sheet1!A81</f>
         <v>SIGA</v>
@@ -17003,24 +17160,26 @@
         <v>11:33:05 AM
 05/27/2022</v>
       </c>
-      <c r="D78" t="str">
-        <f>Sheet1!D81</f>
-        <v>Limit at $11.74</v>
-      </c>
-      <c r="E78" t="str">
-        <f>Sheet1!E81</f>
-        <v xml:space="preserve">Sell 50 Limit at $11.74  </v>
-      </c>
-      <c r="F78" t="str">
-        <f>Sheet1!F81</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G78" t="str">
-        <f>Sheet1!G81</f>
+      <c r="D78" t="s">
+        <v>66</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>849</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="G78" t="s">
+        <v>851</v>
+      </c>
+      <c r="H78" t="s">
+        <v>265</v>
+      </c>
+      <c r="I78">
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f>Sheet1!A82</f>
         <v>SIGA</v>
@@ -17035,24 +17194,26 @@
         <v>11:45:20 AM
 05/27/2022</v>
       </c>
-      <c r="D79" t="str">
-        <f>Sheet1!D82</f>
-        <v>Limit at $12.41</v>
-      </c>
-      <c r="E79" t="str">
-        <f>Sheet1!E82</f>
-        <v xml:space="preserve">Buy 20 Limit at $12.41  </v>
-      </c>
-      <c r="F79" t="str">
-        <f>Sheet1!F82</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G79" t="str">
-        <f>Sheet1!G82</f>
+      <c r="D79" t="s">
+        <v>66</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="G79" t="s">
+        <v>672</v>
+      </c>
+      <c r="H79" t="s">
+        <v>62</v>
+      </c>
+      <c r="I79">
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f>Sheet1!A83</f>
         <v>SIGA</v>
@@ -17067,24 +17228,26 @@
         <v>11:46:18 AM
 05/27/2022</v>
       </c>
-      <c r="D80" t="str">
-        <f>Sheet1!D83</f>
-        <v>Limit at $12.55</v>
-      </c>
-      <c r="E80" t="str">
-        <f>Sheet1!E83</f>
-        <v xml:space="preserve">Buy 10 Limit at $12.55  </v>
-      </c>
-      <c r="F80" t="str">
-        <f>Sheet1!F83</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G80" t="str">
-        <f>Sheet1!G83</f>
+      <c r="D80" t="s">
+        <v>66</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="G80" t="s">
+        <v>855</v>
+      </c>
+      <c r="H80" t="s">
+        <v>270</v>
+      </c>
+      <c r="I80">
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
         <f>Sheet1!A84</f>
         <v>FTCH</v>
@@ -17099,24 +17262,26 @@
         <v>11:58:59 AM
 05/27/2022</v>
       </c>
-      <c r="D81" t="str">
-        <f>Sheet1!D84</f>
-        <v>Limit at $9.73</v>
-      </c>
-      <c r="E81" t="str">
-        <f>Sheet1!E84</f>
-        <v xml:space="preserve">Buy 10 Limit at $9.73  </v>
-      </c>
-      <c r="F81" t="str">
-        <f>Sheet1!F84</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G81" t="str">
-        <f>Sheet1!G84</f>
+      <c r="D81" t="s">
+        <v>272</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="G81" t="s">
+        <v>858</v>
+      </c>
+      <c r="H81" t="s">
+        <v>273</v>
+      </c>
+      <c r="I81">
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
         <f>Sheet1!A85</f>
         <v>FTCH</v>
@@ -17131,24 +17296,26 @@
         <v>11:59:43 AM
 05/27/2022</v>
       </c>
-      <c r="D82" t="str">
-        <f>Sheet1!D85</f>
-        <v>Limit at $9.67</v>
-      </c>
-      <c r="E82" t="str">
-        <f>Sheet1!E85</f>
-        <v xml:space="preserve">Buy 20 Limit at $9.67  </v>
-      </c>
-      <c r="F82" t="str">
-        <f>Sheet1!F85</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G82" t="str">
-        <f>Sheet1!G85</f>
+      <c r="D82" t="s">
+        <v>272</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="G82" t="s">
+        <v>861</v>
+      </c>
+      <c r="H82" t="s">
+        <v>276</v>
+      </c>
+      <c r="I82">
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
         <f>Sheet1!A86</f>
         <v>AVDL</v>
@@ -17163,24 +17330,26 @@
         <v>12:01:16 PM
 05/27/2022</v>
       </c>
-      <c r="D83" t="str">
-        <f>Sheet1!D86</f>
-        <v>Limit at $2.45</v>
-      </c>
-      <c r="E83" t="str">
-        <f>Sheet1!E86</f>
-        <v xml:space="preserve">Buy 20 Limit at $2.45  </v>
-      </c>
-      <c r="F83" t="str">
-        <f>Sheet1!F86</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G83" t="str">
-        <f>Sheet1!G86</f>
+      <c r="D83" t="s">
+        <v>17</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>862</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="G83" t="s">
+        <v>864</v>
+      </c>
+      <c r="H83" t="s">
+        <v>279</v>
+      </c>
+      <c r="I83">
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
         <f>Sheet1!A87</f>
         <v>BB</v>
@@ -17195,24 +17364,26 @@
         <v>12:03:47 PM
 05/27/2022</v>
       </c>
-      <c r="D84" t="str">
-        <f>Sheet1!D87</f>
-        <v>Limit at $6.66</v>
-      </c>
-      <c r="E84" t="str">
-        <f>Sheet1!E87</f>
-        <v xml:space="preserve">Buy 40 Limit at $6.66  </v>
-      </c>
-      <c r="F84" t="str">
-        <f>Sheet1!F87</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G84" t="str">
-        <f>Sheet1!G87</f>
+      <c r="D84" t="s">
+        <v>282</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="G84" t="s">
+        <v>867</v>
+      </c>
+      <c r="H84" t="s">
+        <v>283</v>
+      </c>
+      <c r="I84">
         <v>40</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
         <f>Sheet1!A88</f>
         <v>BB</v>
@@ -17227,24 +17398,26 @@
         <v>12:04:43 PM
 05/27/2022</v>
       </c>
-      <c r="D85" t="str">
-        <f>Sheet1!D88</f>
-        <v>Limit at $6.62</v>
-      </c>
-      <c r="E85" t="str">
-        <f>Sheet1!E88</f>
-        <v xml:space="preserve">Buy 10 Limit at $6.62  </v>
-      </c>
-      <c r="F85" t="str">
-        <f>Sheet1!F88</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G85" t="str">
-        <f>Sheet1!G88</f>
+      <c r="D85" t="s">
+        <v>282</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="G85" t="s">
+        <v>870</v>
+      </c>
+      <c r="H85" t="s">
+        <v>287</v>
+      </c>
+      <c r="I85">
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f>Sheet1!A89</f>
         <v>AVDL</v>
@@ -17259,24 +17432,26 @@
         <v>12:12:34 PM
 05/27/2022</v>
       </c>
-      <c r="D86" t="str">
-        <f>Sheet1!D89</f>
-        <v>Limit at $2.38</v>
-      </c>
-      <c r="E86" t="str">
-        <f>Sheet1!E89</f>
-        <v xml:space="preserve">Sell 70 Limit at $2.38  </v>
-      </c>
-      <c r="F86" t="str">
-        <f>Sheet1!F89</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G86" t="str">
-        <f>Sheet1!G89</f>
+      <c r="D86" t="s">
+        <v>17</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="G86" t="s">
+        <v>873</v>
+      </c>
+      <c r="H86" t="s">
+        <v>290</v>
+      </c>
+      <c r="I86">
         <v>70</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
         <f>Sheet1!A90</f>
         <v>AVDL</v>
@@ -17291,24 +17466,26 @@
         <v>12:24:35 PM
 05/27/2022</v>
       </c>
-      <c r="D87" t="str">
-        <f>Sheet1!D90</f>
-        <v>Limit at $2.28</v>
-      </c>
-      <c r="E87" t="str">
-        <f>Sheet1!E90</f>
-        <v xml:space="preserve">Sell 50 Limit at $2.28  </v>
-      </c>
-      <c r="F87" t="str">
-        <f>Sheet1!F90</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G87" t="str">
-        <f>Sheet1!G90</f>
+      <c r="D87" t="s">
+        <v>17</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>874</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="G87" t="s">
+        <v>876</v>
+      </c>
+      <c r="H87" t="s">
+        <v>295</v>
+      </c>
+      <c r="I87">
         <v>50</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
         <f>Sheet1!A91</f>
         <v>CNCE</v>
@@ -17323,24 +17500,26 @@
         <v>12:25:09 PM
 05/27/2022</v>
       </c>
-      <c r="D88" t="str">
-        <f>Sheet1!D91</f>
-        <v>Limit at $6.83</v>
-      </c>
-      <c r="E88" t="str">
-        <f>Sheet1!E91</f>
-        <v xml:space="preserve">Buy 30 Limit at $6.83  </v>
-      </c>
-      <c r="F88" t="str">
-        <f>Sheet1!F91</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G88" t="str">
-        <f>Sheet1!G91</f>
+      <c r="D88" t="s">
+        <v>298</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="G88" t="s">
+        <v>879</v>
+      </c>
+      <c r="H88" t="s">
+        <v>299</v>
+      </c>
+      <c r="I88">
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
         <f>Sheet1!A92</f>
         <v>CNCE</v>
@@ -17355,24 +17534,26 @@
         <v>12:26:02 PM
 05/27/2022</v>
       </c>
-      <c r="D89" t="str">
-        <f>Sheet1!D92</f>
-        <v>Limit at $6.79</v>
-      </c>
-      <c r="E89" t="str">
-        <f>Sheet1!E92</f>
-        <v xml:space="preserve">Buy 30 Limit at $6.79  </v>
-      </c>
-      <c r="F89" t="str">
-        <f>Sheet1!F92</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G89" t="str">
-        <f>Sheet1!G92</f>
+      <c r="D89" t="s">
+        <v>298</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="G89" t="s">
+        <v>882</v>
+      </c>
+      <c r="H89" t="s">
+        <v>302</v>
+      </c>
+      <c r="I89">
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
         <f>Sheet1!A93</f>
         <v>AVDL</v>
@@ -17387,24 +17568,26 @@
         <v>12:33:03 PM
 05/27/2022</v>
       </c>
-      <c r="D90" t="str">
-        <f>Sheet1!D93</f>
-        <v>Limit at $2.40</v>
-      </c>
-      <c r="E90" t="str">
-        <f>Sheet1!E93</f>
-        <v xml:space="preserve">Buy 50 Limit at $2.40  </v>
-      </c>
-      <c r="F90" t="str">
-        <f>Sheet1!F93</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G90" t="str">
-        <f>Sheet1!G93</f>
+      <c r="D90" t="s">
+        <v>17</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>883</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>884</v>
+      </c>
+      <c r="G90" t="s">
+        <v>885</v>
+      </c>
+      <c r="H90" t="s">
+        <v>305</v>
+      </c>
+      <c r="I90">
         <v>50</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
         <f>Sheet1!A94</f>
         <v>SIGA</v>
@@ -17419,24 +17602,26 @@
         <v>12:45:03 PM
 05/27/2022</v>
       </c>
-      <c r="D91" t="str">
-        <f>Sheet1!D94</f>
-        <v>Limit at $12.73</v>
-      </c>
-      <c r="E91" t="str">
-        <f>Sheet1!E94</f>
-        <v xml:space="preserve">Sell 30 Limit at $12.73  </v>
-      </c>
-      <c r="F91" t="str">
-        <f>Sheet1!F94</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G91" t="str">
-        <f>Sheet1!G94</f>
+      <c r="D91" t="s">
+        <v>66</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="G91" t="s">
+        <v>888</v>
+      </c>
+      <c r="H91" t="s">
+        <v>308</v>
+      </c>
+      <c r="I91">
         <v>30</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
         <f>Sheet1!A95</f>
         <v>SIGA</v>
@@ -17451,24 +17636,26 @@
         <v>12:46:45 PM
 05/27/2022</v>
       </c>
-      <c r="D92" t="str">
-        <f>Sheet1!D95</f>
-        <v>Limit at $12.90</v>
-      </c>
-      <c r="E92" t="str">
-        <f>Sheet1!E95</f>
-        <v xml:space="preserve">Buy 30 Limit at $12.90  </v>
-      </c>
-      <c r="F92" t="str">
-        <f>Sheet1!F95</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G92" t="str">
-        <f>Sheet1!G95</f>
+      <c r="D92" t="s">
+        <v>66</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="G92" t="s">
+        <v>891</v>
+      </c>
+      <c r="H92" t="s">
+        <v>311</v>
+      </c>
+      <c r="I92">
         <v>30</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
         <f>Sheet1!A96</f>
         <v>SIGA</v>
@@ -17483,24 +17670,26 @@
         <v>12:47:49 PM
 05/27/2022</v>
       </c>
-      <c r="D93" t="str">
-        <f>Sheet1!D96</f>
-        <v>Limit at $12.85</v>
-      </c>
-      <c r="E93" t="str">
-        <f>Sheet1!E96</f>
-        <v xml:space="preserve">Sell 30 Limit at $12.85  </v>
-      </c>
-      <c r="F93" t="str">
-        <f>Sheet1!F96</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G93" t="str">
-        <f>Sheet1!G96</f>
+      <c r="D93" t="s">
+        <v>66</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>892</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>893</v>
+      </c>
+      <c r="G93" t="s">
+        <v>894</v>
+      </c>
+      <c r="H93" t="s">
+        <v>314</v>
+      </c>
+      <c r="I93">
         <v>30</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
         <f>Sheet1!A97</f>
         <v>MRNA</v>
@@ -17515,24 +17704,26 @@
         <v>12:50:53 PM
 05/27/2022</v>
       </c>
-      <c r="D94" t="str">
-        <f>Sheet1!D97</f>
-        <v>Limit at $145.85</v>
-      </c>
-      <c r="E94" t="str">
-        <f>Sheet1!E97</f>
-        <v xml:space="preserve">Sell 3 Limit at $145.85  </v>
-      </c>
-      <c r="F94" t="str">
-        <f>Sheet1!F97</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G94" t="str">
-        <f>Sheet1!G97</f>
+      <c r="D94" t="s">
+        <v>182</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>895</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>896</v>
+      </c>
+      <c r="G94" t="s">
+        <v>897</v>
+      </c>
+      <c r="H94" t="s">
+        <v>317</v>
+      </c>
+      <c r="I94">
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
         <f>Sheet1!A98</f>
         <v>NCLH</v>
@@ -17547,24 +17738,26 @@
         <v>12:51:14 PM
 05/27/2022</v>
       </c>
-      <c r="D95" t="str">
-        <f>Sheet1!D98</f>
-        <v>Limit at $16.03</v>
-      </c>
-      <c r="E95" t="str">
-        <f>Sheet1!E98</f>
-        <v xml:space="preserve">Sell 10 Limit at $16.03  </v>
-      </c>
-      <c r="F95" t="str">
-        <f>Sheet1!F98</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G95" t="str">
-        <f>Sheet1!G98</f>
+      <c r="D95" t="s">
+        <v>117</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>899</v>
+      </c>
+      <c r="G95" t="s">
+        <v>900</v>
+      </c>
+      <c r="H95" t="s">
+        <v>321</v>
+      </c>
+      <c r="I95">
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
         <f>Sheet1!A99</f>
         <v>SIGA</v>
@@ -17579,24 +17772,26 @@
         <v>12:52:46 PM
 05/27/2022</v>
       </c>
-      <c r="D96" t="str">
-        <f>Sheet1!D99</f>
-        <v>Limit at $13.85</v>
-      </c>
-      <c r="E96" t="str">
-        <f>Sheet1!E99</f>
-        <v xml:space="preserve">Buy 20 Limit at $13.85  </v>
-      </c>
-      <c r="F96" t="str">
-        <f>Sheet1!F99</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G96" t="str">
-        <f>Sheet1!G99</f>
+      <c r="D96" t="s">
+        <v>66</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="G96" t="s">
+        <v>903</v>
+      </c>
+      <c r="H96" t="s">
+        <v>324</v>
+      </c>
+      <c r="I96">
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
         <f>Sheet1!A100</f>
         <v>FTCH</v>
@@ -17611,24 +17806,26 @@
         <v>12:56:30 PM
 05/27/2022</v>
       </c>
-      <c r="D97" t="str">
-        <f>Sheet1!D100</f>
-        <v>Limit at $9.65</v>
-      </c>
-      <c r="E97" t="str">
-        <f>Sheet1!E100</f>
-        <v xml:space="preserve">Sell 30 Limit at $9.65  </v>
-      </c>
-      <c r="F97" t="str">
-        <f>Sheet1!F100</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G97" t="str">
-        <f>Sheet1!G100</f>
+      <c r="D97" t="s">
+        <v>272</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="G97" t="s">
+        <v>906</v>
+      </c>
+      <c r="H97" t="s">
+        <v>327</v>
+      </c>
+      <c r="I97">
         <v>30</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
         <f>Sheet1!A101</f>
         <v>MRNA</v>
@@ -17643,24 +17840,26 @@
         <v>12:57:28 PM
 05/27/2022</v>
       </c>
-      <c r="D98" t="str">
-        <f>Sheet1!D101</f>
-        <v>Limit at $146.27</v>
-      </c>
-      <c r="E98" t="str">
-        <f>Sheet1!E101</f>
-        <v xml:space="preserve">Sell 3 Limit at $146.27  </v>
-      </c>
-      <c r="F98" t="str">
-        <f>Sheet1!F101</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G98" t="str">
-        <f>Sheet1!G101</f>
+      <c r="D98" t="s">
+        <v>182</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>907</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>908</v>
+      </c>
+      <c r="G98" t="s">
+        <v>909</v>
+      </c>
+      <c r="H98" t="s">
+        <v>330</v>
+      </c>
+      <c r="I98">
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
         <f>Sheet1!A102</f>
         <v>MRVL</v>
@@ -17675,24 +17874,26 @@
         <v>12:57:58 PM
 05/27/2022</v>
       </c>
-      <c r="D99" t="str">
-        <f>Sheet1!D102</f>
-        <v>Limit at $59.70</v>
-      </c>
-      <c r="E99" t="str">
-        <f>Sheet1!E102</f>
-        <v xml:space="preserve">Sell 1 Limit at $59.70  </v>
-      </c>
-      <c r="F99" t="str">
-        <f>Sheet1!F102</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G99" t="str">
-        <f>Sheet1!G102</f>
+      <c r="D99" t="s">
+        <v>192</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>910</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="G99" t="s">
+        <v>912</v>
+      </c>
+      <c r="H99" t="s">
+        <v>333</v>
+      </c>
+      <c r="I99">
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
         <f>Sheet1!A103</f>
         <v>AMC</v>
@@ -17707,24 +17908,26 @@
         <v>12:58:46 PM
 05/27/2022</v>
       </c>
-      <c r="D100" t="str">
-        <f>Sheet1!D103</f>
-        <v>Limit at $13.29</v>
-      </c>
-      <c r="E100" t="str">
-        <f>Sheet1!E103</f>
-        <v xml:space="preserve">Sell 20 Limit at $13.29  </v>
-      </c>
-      <c r="F100" t="str">
-        <f>Sheet1!F103</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G100" t="str">
-        <f>Sheet1!G103</f>
+      <c r="D100" t="s">
+        <v>57</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="G100" t="s">
+        <v>915</v>
+      </c>
+      <c r="H100" t="s">
+        <v>336</v>
+      </c>
+      <c r="I100">
         <v>20</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A101" t="str">
         <f>Sheet1!A104</f>
         <v>TSLA</v>
@@ -17739,24 +17942,26 @@
         <v>12:59:29 PM
 05/27/2022</v>
       </c>
-      <c r="D101" t="str">
-        <f>Sheet1!D104</f>
-        <v>Limit at $750.60</v>
-      </c>
-      <c r="E101" t="str">
-        <f>Sheet1!E104</f>
-        <v xml:space="preserve">Sell 1 Limit at $750.60  </v>
-      </c>
-      <c r="F101" t="str">
-        <f>Sheet1!F104</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G101" t="str">
-        <f>Sheet1!G104</f>
+      <c r="D101" t="s">
+        <v>109</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>917</v>
+      </c>
+      <c r="G101" t="s">
+        <v>918</v>
+      </c>
+      <c r="H101" t="s">
+        <v>339</v>
+      </c>
+      <c r="I101">
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" t="str">
         <f>Sheet1!A105</f>
         <v>SHOP</v>
@@ -17771,24 +17976,26 @@
         <v>12:59:44 PM
 05/27/2022</v>
       </c>
-      <c r="D102" t="str">
-        <f>Sheet1!D105</f>
-        <v>Limit at $365.12</v>
-      </c>
-      <c r="E102" t="str">
-        <f>Sheet1!E105</f>
-        <v xml:space="preserve">Sell 1 Limit at $365.12  </v>
-      </c>
-      <c r="F102" t="str">
-        <f>Sheet1!F105</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G102" t="str">
-        <f>Sheet1!G105</f>
+      <c r="D102" t="s">
+        <v>147</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="G102" t="s">
+        <v>921</v>
+      </c>
+      <c r="H102" t="s">
+        <v>342</v>
+      </c>
+      <c r="I102">
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A103" t="str">
         <f>Sheet1!A106</f>
         <v>SQ</v>
@@ -17803,24 +18010,26 @@
         <v>01:01:41 PM
 05/27/2022</v>
       </c>
-      <c r="D103" t="str">
-        <f>Sheet1!D106</f>
-        <v>Limit at $89.46</v>
-      </c>
-      <c r="E103" t="str">
-        <f>Sheet1!E106</f>
-        <v xml:space="preserve">Sell 1 Limit at $89.46  </v>
-      </c>
-      <c r="F103" t="str">
-        <f>Sheet1!F106</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G103" t="str">
-        <f>Sheet1!G106</f>
+      <c r="D103" t="s">
+        <v>223</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>923</v>
+      </c>
+      <c r="G103" t="s">
+        <v>924</v>
+      </c>
+      <c r="H103" t="s">
+        <v>345</v>
+      </c>
+      <c r="I103">
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A104" t="str">
         <f>Sheet1!A107</f>
         <v>CNCE</v>
@@ -17835,24 +18044,26 @@
         <v>01:05:01 PM
 05/27/2022</v>
       </c>
-      <c r="D104" t="str">
-        <f>Sheet1!D107</f>
-        <v>Stop Loss at $6.40</v>
-      </c>
-      <c r="E104" t="str">
-        <f>Sheet1!E107</f>
-        <v xml:space="preserve">Sell 60 Stop Loss at $6.40  </v>
-      </c>
-      <c r="F104" t="str">
-        <f>Sheet1!F107</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G104" t="str">
-        <f>Sheet1!G107</f>
+      <c r="D104" t="s">
+        <v>298</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="G104" t="s">
+        <v>927</v>
+      </c>
+      <c r="H104" t="s">
+        <v>348</v>
+      </c>
+      <c r="I104">
         <v>60</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
         <f>Sheet1!A108</f>
         <v>FB</v>
@@ -17867,24 +18078,26 @@
         <v>01:05:40 PM
 05/27/2022</v>
       </c>
-      <c r="D105" t="str">
-        <f>Sheet1!D108</f>
-        <v>Limit at $193.84</v>
-      </c>
-      <c r="E105" t="str">
-        <f>Sheet1!E108</f>
-        <v xml:space="preserve">Sell 5 Limit at $193.84  </v>
-      </c>
-      <c r="F105" t="str">
-        <f>Sheet1!F108</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G105" t="str">
-        <f>Sheet1!G108</f>
+      <c r="D105" t="s">
+        <v>129</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>929</v>
+      </c>
+      <c r="G105" t="s">
+        <v>930</v>
+      </c>
+      <c r="H105" t="s">
+        <v>353</v>
+      </c>
+      <c r="I105">
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A106" t="str">
         <f>Sheet1!A109</f>
         <v>AMD</v>
@@ -17899,24 +18112,26 @@
         <v>01:06:38 PM
 05/27/2022</v>
       </c>
-      <c r="D106" t="str">
-        <f>Sheet1!D109</f>
-        <v>Limit at $100.94</v>
-      </c>
-      <c r="E106" t="str">
-        <f>Sheet1!E109</f>
-        <v xml:space="preserve">Sell 5 Limit at $100.94  </v>
-      </c>
-      <c r="F106" t="str">
-        <f>Sheet1!F109</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G106" t="str">
-        <f>Sheet1!G109</f>
+      <c r="D106" t="s">
+        <v>105</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="G106" t="s">
+        <v>933</v>
+      </c>
+      <c r="H106" t="s">
+        <v>357</v>
+      </c>
+      <c r="I106">
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A107" t="str">
         <f>Sheet1!A110</f>
         <v>SIGA</v>
@@ -17931,24 +18146,26 @@
         <v>01:08:25 PM
 05/27/2022</v>
       </c>
-      <c r="D107" t="str">
-        <f>Sheet1!D110</f>
-        <v>Limit at $14.37</v>
-      </c>
-      <c r="E107" t="str">
-        <f>Sheet1!E110</f>
-        <v xml:space="preserve">Sell 20 Limit at $14.37  </v>
-      </c>
-      <c r="F107" t="str">
-        <f>Sheet1!F110</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G107" t="str">
-        <f>Sheet1!G110</f>
+      <c r="D107" t="s">
+        <v>66</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>934</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="G107" t="s">
+        <v>936</v>
+      </c>
+      <c r="H107" t="s">
+        <v>360</v>
+      </c>
+      <c r="I107">
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
         <f>Sheet1!A111</f>
         <v>SHOP</v>
@@ -17963,24 +18180,26 @@
         <v>01:09:04 PM
 05/27/2022</v>
       </c>
-      <c r="D108" t="str">
-        <f>Sheet1!D111</f>
-        <v>Limit at $364.30</v>
-      </c>
-      <c r="E108" t="str">
-        <f>Sheet1!E111</f>
-        <v xml:space="preserve">Sell 1 Limit at $364.30  </v>
-      </c>
-      <c r="F108" t="str">
-        <f>Sheet1!F111</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G108" t="str">
-        <f>Sheet1!G111</f>
+      <c r="D108" t="s">
+        <v>147</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="G108" t="s">
+        <v>939</v>
+      </c>
+      <c r="H108" t="s">
+        <v>363</v>
+      </c>
+      <c r="I108">
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A109" t="str">
         <f>Sheet1!A112</f>
         <v>NVDA</v>
@@ -17995,24 +18214,26 @@
         <v>01:09:35 PM
 05/27/2022</v>
       </c>
-      <c r="D109" t="str">
-        <f>Sheet1!D112</f>
-        <v>Limit at $185.74</v>
-      </c>
-      <c r="E109" t="str">
-        <f>Sheet1!E112</f>
-        <v xml:space="preserve">Sell 5 Limit at $185.74  </v>
-      </c>
-      <c r="F109" t="str">
-        <f>Sheet1!F112</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G109" t="str">
-        <f>Sheet1!G112</f>
+      <c r="D109" t="s">
+        <v>113</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>940</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>941</v>
+      </c>
+      <c r="G109" t="s">
+        <v>942</v>
+      </c>
+      <c r="H109" t="s">
+        <v>366</v>
+      </c>
+      <c r="I109">
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
         <f>Sheet1!A113</f>
         <v>TSLA</v>
@@ -18027,24 +18248,26 @@
         <v>01:10:17 PM
 05/27/2022</v>
       </c>
-      <c r="D110" t="str">
-        <f>Sheet1!D113</f>
-        <v>Limit at $751.56</v>
-      </c>
-      <c r="E110" t="str">
-        <f>Sheet1!E113</f>
-        <v xml:space="preserve">Sell 1 Limit at $751.56  </v>
-      </c>
-      <c r="F110" t="str">
-        <f>Sheet1!F113</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G110" t="str">
-        <f>Sheet1!G113</f>
+      <c r="D110" t="s">
+        <v>109</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>944</v>
+      </c>
+      <c r="G110" t="s">
+        <v>945</v>
+      </c>
+      <c r="H110" t="s">
+        <v>369</v>
+      </c>
+      <c r="I110">
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A111" t="str">
         <f>Sheet1!A114</f>
         <v>BABA</v>
@@ -18059,24 +18282,26 @@
         <v>01:10:40 PM
 05/27/2022</v>
       </c>
-      <c r="D111" t="str">
-        <f>Sheet1!D114</f>
-        <v>Limit at $93.09</v>
-      </c>
-      <c r="E111" t="str">
-        <f>Sheet1!E114</f>
-        <v xml:space="preserve">Sell 4 Limit at $93.09  </v>
-      </c>
-      <c r="F111" t="str">
-        <f>Sheet1!F114</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G111" t="str">
-        <f>Sheet1!G114</f>
+      <c r="D111" t="s">
+        <v>154</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>947</v>
+      </c>
+      <c r="G111" t="s">
+        <v>948</v>
+      </c>
+      <c r="H111" t="s">
+        <v>372</v>
+      </c>
+      <c r="I111">
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A112" t="str">
         <f>Sheet1!A115</f>
         <v>MSFT</v>
@@ -18091,24 +18316,26 @@
         <v>01:11:18 PM
 05/27/2022</v>
       </c>
-      <c r="D112" t="str">
-        <f>Sheet1!D115</f>
-        <v>Limit at $271.59</v>
-      </c>
-      <c r="E112" t="str">
-        <f>Sheet1!E115</f>
-        <v xml:space="preserve">Sell 6 Limit at $271.59  </v>
-      </c>
-      <c r="F112" t="str">
-        <f>Sheet1!F115</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G112" t="str">
-        <f>Sheet1!G115</f>
+      <c r="D112" t="s">
+        <v>100</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>949</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="G112" t="s">
+        <v>951</v>
+      </c>
+      <c r="H112" t="s">
+        <v>377</v>
+      </c>
+      <c r="I112">
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A113" t="str">
         <f>Sheet1!A116</f>
         <v>NVDA</v>
@@ -18123,24 +18350,26 @@
         <v>01:11:48 PM
 05/27/2022</v>
       </c>
-      <c r="D113" t="str">
-        <f>Sheet1!D116</f>
-        <v>Limit at $185.78</v>
-      </c>
-      <c r="E113" t="str">
-        <f>Sheet1!E116</f>
-        <v xml:space="preserve">Sell 3 Limit at $185.78  </v>
-      </c>
-      <c r="F113" t="str">
-        <f>Sheet1!F116</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G113" t="str">
-        <f>Sheet1!G116</f>
+      <c r="D113" t="s">
+        <v>113</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>952</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>953</v>
+      </c>
+      <c r="G113" t="s">
+        <v>954</v>
+      </c>
+      <c r="H113" t="s">
+        <v>382</v>
+      </c>
+      <c r="I113">
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A114" t="str">
         <f>Sheet1!A117</f>
         <v>TSLA</v>
@@ -18155,24 +18384,26 @@
         <v>01:12:26 PM
 05/27/2022</v>
       </c>
-      <c r="D114" t="str">
-        <f>Sheet1!D117</f>
-        <v>Limit at $752.78</v>
-      </c>
-      <c r="E114" t="str">
-        <f>Sheet1!E117</f>
-        <v xml:space="preserve">Sell 1 Limit at $752.78  </v>
-      </c>
-      <c r="F114" t="str">
-        <f>Sheet1!F117</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G114" t="str">
-        <f>Sheet1!G117</f>
+      <c r="D114" t="s">
+        <v>109</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>955</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="G114" t="s">
+        <v>957</v>
+      </c>
+      <c r="H114" t="s">
+        <v>385</v>
+      </c>
+      <c r="I114">
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A115" t="str">
         <f>Sheet1!A118</f>
         <v>BB</v>
@@ -18187,24 +18418,26 @@
         <v>01:12:55 PM
 05/27/2022</v>
       </c>
-      <c r="D115" t="str">
-        <f>Sheet1!D118</f>
-        <v>Limit at $6.67</v>
-      </c>
-      <c r="E115" t="str">
-        <f>Sheet1!E118</f>
-        <v xml:space="preserve">Sell 50 Limit at $6.67  </v>
-      </c>
-      <c r="F115" t="str">
-        <f>Sheet1!F118</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G115" t="str">
-        <f>Sheet1!G118</f>
+      <c r="D115" t="s">
+        <v>282</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>958</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="G115" t="s">
+        <v>960</v>
+      </c>
+      <c r="H115" t="s">
+        <v>388</v>
+      </c>
+      <c r="I115">
         <v>50</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A116" t="str">
         <f>Sheet1!A119</f>
         <v>AVDL</v>
@@ -18219,20 +18452,22 @@
         <v>01:20:54 PM
 05/27/2022</v>
       </c>
-      <c r="D116" t="str">
-        <f>Sheet1!D119</f>
-        <v>Limit at $2.30</v>
-      </c>
-      <c r="E116" t="str">
-        <f>Sheet1!E119</f>
-        <v xml:space="preserve">Sell 50 Limit at $2.30  </v>
-      </c>
-      <c r="F116" t="str">
-        <f>Sheet1!F119</f>
-        <v>ROLLOVER IRA (110992950)</v>
-      </c>
-      <c r="G116" t="str">
-        <f>Sheet1!G119</f>
+      <c r="D116" t="s">
+        <v>17</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>961</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>962</v>
+      </c>
+      <c r="G116" t="s">
+        <v>823</v>
+      </c>
+      <c r="H116" t="s">
+        <v>391</v>
+      </c>
+      <c r="I116">
         <v>50</v>
       </c>
     </row>

</xml_diff>